<commit_message>
Organisation des fichiers dans le repo
</commit_message>
<xml_diff>
--- a/Journaux de travail/Journal_PedroPinto.xlsx
+++ b/Journaux de travail/Journal_PedroPinto.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -185,6 +185,12 @@
 -Creation de la fonction allent chercher les données insérées dans les annonces
 -Création de la fonction permetant l'organisation dans le controleur
 -Ajout de la page submitAdd dans l'index en metode POST</t>
+  </si>
+  <si>
+    <t>Ajout dans la page d'acceuile 
+-CSS réorganisé 
+-Mis a jour de la version de Bootstrap + 
+Réparation des conflits</t>
   </si>
 </sst>
 </file>
@@ -931,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,15 +1295,25 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
+    <row r="20" spans="2:7" ht="57" x14ac:dyDescent="0.25">
+      <c r="B20" s="8">
+        <v>44258</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="F20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="11"/>
+      <c r="G20" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>

</xml_diff>

<commit_message>
Journal de travaile + Nouveau CDC
</commit_message>
<xml_diff>
--- a/Journaux de travail/Journal_PedroPinto.xlsx
+++ b/Journaux de travail/Journal_PedroPinto.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -161,10 +161,6 @@
     <t>10H00</t>
   </si>
   <si>
-    <t>Retour sur la fin du sprinte 1
-et le début du sprinte 2 avec  Mr.Chavais et Simon Cuany</t>
-  </si>
-  <si>
     <t>Rédaction de l'analyse dans la documentationb 
 avec Simon Cuany</t>
   </si>
@@ -212,6 +208,13 @@
   </si>
   <si>
     <t>Rédaction de l'integralité de la conseption dans le CDC + Suppresion de librairies inutiles</t>
+  </si>
+  <si>
+    <t>Retour sur la fin du sprinte 1
+et le début du sprinte 2 avec  Mr.Chaveys et Simon Cuany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redaction du CDC </t>
   </si>
 </sst>
 </file>
@@ -958,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,7 +1239,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B16" s="8">
         <v>44256</v>
       </c>
@@ -1253,7 +1256,7 @@
         <v>10</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="42.75" x14ac:dyDescent="0.25">
@@ -1273,10 +1276,10 @@
         <v>10</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="57" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <v>44256</v>
       </c>
@@ -1293,7 +1296,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
@@ -1304,16 +1307,16 @@
         <v>7</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="F19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="57" x14ac:dyDescent="0.25">
@@ -1333,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="28.5" x14ac:dyDescent="0.25">
@@ -1353,7 +1356,7 @@
         <v>10</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="28.5" x14ac:dyDescent="0.25">
@@ -1373,7 +1376,7 @@
         <v>10</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="28.5" x14ac:dyDescent="0.25">
@@ -1381,10 +1384,10 @@
         <v>44274</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>34</v>
@@ -1393,7 +1396,7 @@
         <v>10</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="42.75" x14ac:dyDescent="0.25">
@@ -1407,24 +1410,34 @@
         <v>7</v>
       </c>
       <c r="E24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
+      <c r="B25" s="8">
+        <v>44277</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="F25" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G25" s="12"/>
+      <c r="G25" s="12" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>

</xml_diff>